<commit_message>
update missing gender data and charts
</commit_message>
<xml_diff>
--- a/02_programs/Fig2 SDG5 coverage_data_updated.xlsx
+++ b/02_programs/Fig2 SDG5 coverage_data_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB469649\Documents\Github\Missing-SDG-Gender-Indicators\02_programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5FB550-FDB4-4BBF-B86D-E603D03D6B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88591C35-2AEC-4367-9598-404844CFEE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2ED9C81-B963-4F24-A64E-BC89C20E589A}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -146,7 +146,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -186,14 +186,11 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Share of countries</c:v>
-          </c:tx>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent5"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -203,10 +200,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -239,55 +236,67 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Sheet1!$D$2:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>1.0999999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>2.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>5.52</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>9.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>44</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24</c:v>
+                  <c:v>17.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>9.94</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>7.1800000000000006</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>3.3099999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.55199999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8020-4864-8845-99992ACE98C0}"/>
+              <c16:uniqueId val="{00000000-E75A-4CF2-ACD5-2967968D0764}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -303,6 +312,192 @@
         <c:overlap val="-27"/>
         <c:axId val="162115855"/>
         <c:axId val="162113359"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent6"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$2:$C$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>1.0999999999999999E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2.76E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5.5199999999999999E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>9.3899999999999997E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.21</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.215</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.17699999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>9.9400000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>7.1800000000000003E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>3.3099999999999997E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>5.5199999999999997E-3</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-8020-4864-8845-99992ACE98C0}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:catAx>
         <c:axId val="162115855"/>
@@ -559,13 +754,10 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1105,15 +1297,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>536575</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>488950</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>231775</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>73025</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1439,10 +1631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7CED299-6DF9-4ED3-851E-7BE763957497}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1460,10 +1652,14 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
-        <v>1.66E-2</v>
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D2">
+        <f>100*C2</f>
+        <v>1.0999999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1471,14 +1667,18 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
-        <v>1.66E-2</v>
+        <v>2.76E-2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D14" si="0">100*C3</f>
+        <v>2.76</v>
       </c>
       <c r="E3">
         <f>SUM(B2:B5)</f>
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1486,10 +1686,14 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2">
-        <v>7.7299999999999994E-2</v>
+        <v>5.5199999999999999E-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>5.52</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1497,10 +1701,14 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2">
-        <v>0.11600000000000001</v>
+        <v>9.3899999999999997E-2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>9.39</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1508,10 +1716,14 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2">
-        <v>0.221</v>
+        <v>0.21</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1519,10 +1731,14 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2">
-        <v>0.24299999999999999</v>
+        <v>0.215</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>21.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1530,10 +1746,14 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2">
-        <v>0.13300000000000001</v>
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>17.7</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1541,10 +1761,14 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2">
-        <v>0.11600000000000001</v>
+        <v>9.9400000000000002E-2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>9.94</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1552,10 +1776,14 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2">
-        <v>4.9700000000000001E-2</v>
+        <v>7.1800000000000003E-2</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>7.1800000000000006</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1563,10 +1791,14 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2">
-        <v>5.5199999999999997E-3</v>
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>3.3099999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1574,20 +1806,54 @@
         <v>10</v>
       </c>
       <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
         <v>1</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C14" s="2">
         <v>5.5199999999999997E-3</v>
       </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.55199999999999994</v>
+      </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <f>SUM(B2:B12)</f>
+    <row r="15" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f>SUM(B2:B14)</f>
         <v>181</v>
       </c>
-      <c r="C13" s="5">
-        <f>SUM(C2:C12)</f>
-        <v>1.00024</v>
+      <c r="C15" s="5">
+        <f>SUM(C2:C14)</f>
+        <v>0.99951999999999985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>